<commit_message>
Updated texts database preparation files
</commit_message>
<xml_diff>
--- a/data-raw/texts/AGR_TXT/DESTA_TXT.xlsx
+++ b/data-raw/texts/AGR_TXT/DESTA_TXT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaeltan/Documents/GitHub/manytrade/data-raw/texts/AGR_TXT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B749DF9-058B-4D48-B875-6EE1E70AE032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598393E2-3DD9-A047-9FEE-5927A9F5DA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{2EBF81AD-632B-854A-A9EC-C64523CEF580}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{2EBF81AD-632B-854A-A9EC-C64523CEF580}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5731,9 +5731,6 @@
     <t>CHL-TUR[NA]_2009O</t>
   </si>
   <si>
-    <t>base</t>
-  </si>
-  <si>
     <t>url2</t>
   </si>
   <si>
@@ -5846,6 +5843,9 @@
   </si>
   <si>
     <t>http://www.sice.oas.org/Trade/colpan/colpan_s1.asp</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -6234,9 +6234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{124AB8FC-2BA3-0047-AE15-0F0E5C910EBE}">
   <dimension ref="A1:K797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A491" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I495" sqref="I495"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A642" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I655" sqref="I655"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6273,10 +6273,10 @@
         <v>1372</v>
       </c>
       <c r="H1" t="s">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="I1" t="s">
-        <v>1891</v>
+        <v>1929</v>
       </c>
       <c r="J1" t="s">
         <v>1376</v>
@@ -6819,10 +6819,10 @@
         <v>680</v>
       </c>
       <c r="I25" t="s">
-        <v>1904</v>
+        <v>1903</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>1903</v>
+        <v>1902</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -7384,10 +7384,10 @@
         <v>901</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>1894</v>
+        <v>1893</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>1893</v>
+        <v>1892</v>
       </c>
       <c r="I51" s="3"/>
     </row>
@@ -7812,10 +7812,10 @@
         <v>985</v>
       </c>
       <c r="G70" s="9" t="s">
-        <v>1896</v>
+        <v>1895</v>
       </c>
       <c r="H70" s="9" t="s">
-        <v>1895</v>
+        <v>1894</v>
       </c>
       <c r="I70" s="2"/>
     </row>
@@ -8743,10 +8743,10 @@
         <v>302</v>
       </c>
       <c r="G111" s="10" t="s">
-        <v>1898</v>
+        <v>1897</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>1897</v>
+        <v>1896</v>
       </c>
       <c r="I111" s="3"/>
     </row>
@@ -8770,10 +8770,10 @@
         <v>317</v>
       </c>
       <c r="G112" s="10" t="s">
-        <v>1900</v>
+        <v>1899</v>
       </c>
       <c r="H112" s="11" t="s">
-        <v>1899</v>
+        <v>1898</v>
       </c>
       <c r="I112" s="3"/>
     </row>
@@ -8797,10 +8797,10 @@
         <v>322</v>
       </c>
       <c r="G113" s="10" t="s">
+        <v>1900</v>
+      </c>
+      <c r="H113" s="11" t="s">
         <v>1901</v>
-      </c>
-      <c r="H113" s="11" t="s">
-        <v>1902</v>
       </c>
       <c r="I113" s="3"/>
     </row>
@@ -9183,7 +9183,7 @@
         <v>1641</v>
       </c>
       <c r="J130" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.2">
@@ -10032,7 +10032,7 @@
         <v>144</v>
       </c>
       <c r="G165" t="s">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="K165" t="s">
         <v>1375</v>
@@ -10058,7 +10058,7 @@
         <v>251</v>
       </c>
       <c r="G166" t="s">
-        <v>1922</v>
+        <v>1921</v>
       </c>
       <c r="K166" t="s">
         <v>1375</v>
@@ -10179,7 +10179,7 @@
         <v>421</v>
       </c>
       <c r="G171" t="s">
-        <v>1923</v>
+        <v>1922</v>
       </c>
       <c r="K171" t="s">
         <v>1375</v>
@@ -10205,7 +10205,7 @@
         <v>480</v>
       </c>
       <c r="G172" t="s">
-        <v>1924</v>
+        <v>1923</v>
       </c>
       <c r="K172" t="s">
         <v>1375</v>
@@ -10303,7 +10303,7 @@
         <v>635</v>
       </c>
       <c r="G176" t="s">
-        <v>1925</v>
+        <v>1924</v>
       </c>
       <c r="K176" t="s">
         <v>1375</v>
@@ -10898,7 +10898,7 @@
         <v>681</v>
       </c>
       <c r="G202" t="s">
-        <v>1926</v>
+        <v>1925</v>
       </c>
       <c r="K202" t="s">
         <v>1375</v>
@@ -10924,7 +10924,7 @@
         <v>34</v>
       </c>
       <c r="G203" t="s">
-        <v>1927</v>
+        <v>1926</v>
       </c>
       <c r="K203" t="s">
         <v>1375</v>
@@ -10970,7 +10970,7 @@
         <v>476</v>
       </c>
       <c r="G205" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="K205" t="s">
         <v>1375</v>
@@ -12303,7 +12303,7 @@
         <v>240</v>
       </c>
       <c r="G264" t="s">
-        <v>1929</v>
+        <v>1928</v>
       </c>
       <c r="K264" t="s">
         <v>1375</v>
@@ -12593,7 +12593,7 @@
         <v>1706</v>
       </c>
       <c r="J277" t="s">
-        <v>1906</v>
+        <v>1905</v>
       </c>
     </row>
     <row r="278" spans="1:11" x14ac:dyDescent="0.2">
@@ -12723,7 +12723,7 @@
         <v>172</v>
       </c>
       <c r="G282" t="s">
-        <v>1907</v>
+        <v>1906</v>
       </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.2">
@@ -13004,7 +13004,7 @@
       <c r="F294">
         <v>464</v>
       </c>
-      <c r="G294" t="s">
+      <c r="I294" t="s">
         <v>1718</v>
       </c>
       <c r="K294" t="s">
@@ -13909,7 +13909,7 @@
         <v>123</v>
       </c>
       <c r="G335" t="s">
-        <v>1908</v>
+        <v>1907</v>
       </c>
       <c r="K335" t="s">
         <v>1375</v>
@@ -13955,7 +13955,7 @@
         <v>209</v>
       </c>
       <c r="G337" t="s">
-        <v>1909</v>
+        <v>1908</v>
       </c>
       <c r="K337" t="s">
         <v>1375</v>
@@ -14170,7 +14170,7 @@
         <v>1734</v>
       </c>
       <c r="J347" t="s">
-        <v>1910</v>
+        <v>1909</v>
       </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.2">
@@ -14623,7 +14623,7 @@
         <v>1738</v>
       </c>
       <c r="J368" t="s">
-        <v>1911</v>
+        <v>1910</v>
       </c>
     </row>
     <row r="369" spans="1:7" x14ac:dyDescent="0.2">
@@ -15210,7 +15210,7 @@
         <v>1742</v>
       </c>
       <c r="J396" t="s">
-        <v>1912</v>
+        <v>1911</v>
       </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.2">
@@ -15831,7 +15831,7 @@
       <c r="F424">
         <v>612</v>
       </c>
-      <c r="G424" t="s">
+      <c r="I424" t="s">
         <v>1748</v>
       </c>
       <c r="K424" t="s">
@@ -16531,7 +16531,7 @@
         <v>185</v>
       </c>
       <c r="G456" s="10" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="H456" s="3"/>
       <c r="I456" s="3"/>
@@ -17249,7 +17249,7 @@
         <v>25</v>
       </c>
       <c r="G489" t="s">
-        <v>1914</v>
+        <v>1913</v>
       </c>
       <c r="K489" t="s">
         <v>1375</v>
@@ -17880,8 +17880,8 @@
       <c r="F517">
         <v>606</v>
       </c>
-      <c r="G517" t="s">
-        <v>1915</v>
+      <c r="G517" s="1" t="s">
+        <v>1914</v>
       </c>
       <c r="K517" t="s">
         <v>1375</v>
@@ -18084,7 +18084,7 @@
       <c r="F526">
         <v>291</v>
       </c>
-      <c r="G526" t="s">
+      <c r="I526" t="s">
         <v>1767</v>
       </c>
     </row>
@@ -18107,7 +18107,7 @@
       <c r="F527">
         <v>399</v>
       </c>
-      <c r="G527" t="s">
+      <c r="G527" s="1" t="s">
         <v>1409</v>
       </c>
     </row>
@@ -18256,7 +18256,7 @@
       <c r="F534">
         <v>67</v>
       </c>
-      <c r="G534" t="s">
+      <c r="I534" t="s">
         <v>1410</v>
       </c>
     </row>
@@ -18279,7 +18279,7 @@
       <c r="F535">
         <v>67</v>
       </c>
-      <c r="G535" t="s">
+      <c r="I535" t="s">
         <v>1410</v>
       </c>
     </row>
@@ -18372,7 +18372,7 @@
         <v>239</v>
       </c>
       <c r="G539" s="10" t="s">
-        <v>1916</v>
+        <v>1915</v>
       </c>
       <c r="H539" s="3"/>
       <c r="I539" s="3"/>
@@ -18534,7 +18534,7 @@
       <c r="F546">
         <v>812</v>
       </c>
-      <c r="G546" t="s">
+      <c r="I546" t="s">
         <v>1414</v>
       </c>
       <c r="K546" t="s">
@@ -19361,7 +19361,7 @@
       <c r="F582">
         <v>979</v>
       </c>
-      <c r="G582" t="s">
+      <c r="G582" s="1" t="s">
         <v>1420</v>
       </c>
     </row>
@@ -19523,7 +19523,7 @@
         <v>821</v>
       </c>
       <c r="G589" t="s">
-        <v>1917</v>
+        <v>1916</v>
       </c>
       <c r="K589" t="s">
         <v>1375</v>
@@ -20058,12 +20058,12 @@
         <v>831</v>
       </c>
       <c r="G612" s="10" t="s">
-        <v>1918</v>
+        <v>1917</v>
       </c>
       <c r="H612" s="5"/>
       <c r="I612" s="5"/>
     </row>
-    <row r="613" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="613" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A613" t="s">
         <v>1097</v>
       </c>
@@ -20083,7 +20083,7 @@
         <v>831</v>
       </c>
       <c r="G613" s="5" t="s">
-        <v>1919</v>
+        <v>1918</v>
       </c>
       <c r="H613" s="5"/>
       <c r="I613" s="5"/>
@@ -20574,7 +20574,7 @@
         <v>852</v>
       </c>
       <c r="G634" t="s">
-        <v>1920</v>
+        <v>1919</v>
       </c>
     </row>
     <row r="635" spans="1:7" x14ac:dyDescent="0.2">
@@ -21056,7 +21056,7 @@
       <c r="F655">
         <v>1000</v>
       </c>
-      <c r="G655" t="s">
+      <c r="I655" t="s">
         <v>1783</v>
       </c>
     </row>
@@ -24113,6 +24113,9 @@
     <hyperlink ref="G113" r:id="rId15" xr:uid="{AE5C3B5F-2C7E-C74F-A110-626835218BF1}"/>
     <hyperlink ref="G456" r:id="rId16" xr:uid="{2C8277D6-A572-AD43-8A2D-FA764DD3C3D0}"/>
     <hyperlink ref="G539" r:id="rId17" xr:uid="{55572991-7303-2D4B-A2D1-8810996DE7B2}"/>
+    <hyperlink ref="G517" r:id="rId18" xr:uid="{19B12918-FB4D-6D46-AFF3-5853CB1999A8}"/>
+    <hyperlink ref="G527" r:id="rId19" xr:uid="{E0853028-ED92-FD4A-8736-3824E1D9D21F}"/>
+    <hyperlink ref="G582" r:id="rId20" xr:uid="{3A706D3E-A377-8842-B6BC-F1E555C793B0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>